<commit_message>
resources(tdupe) : [] add brands reference
</commit_message>
<xml_diff>
--- a/resources/physics/tdupe/workingCopy.xlsx
+++ b/resources/physics/tdupe/workingCopy.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="carlist" sheetId="1" r:id="rId1"/>
     <sheet name="cameras" sheetId="2" r:id="rId2"/>
     <sheet name="hud" sheetId="3" r:id="rId3"/>
     <sheet name="rims" sheetId="4" r:id="rId4"/>
+    <sheet name="brandNames" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">brandNames!$A$1:$B$377</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">cameras!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">carlist!$A$1:$B$300</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">hud!$A$1:$B$267</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">rims!$A$1:$B$299</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="2634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3882" uniqueCount="3009">
   <si>
     <t>Reference</t>
   </si>
@@ -7930,19 +7932,1151 @@
   </si>
   <si>
     <t>000034001</t>
+  </si>
+  <si>
+    <t>Mega</t>
+  </si>
+  <si>
+    <t>Mercedes-benz 1920</t>
+  </si>
+  <si>
+    <t>Mercedes-benz 1930</t>
+  </si>
+  <si>
+    <t>Mercedes-benz 1940</t>
+  </si>
+  <si>
+    <t>Messerschmitt</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>Monica</t>
+  </si>
+  <si>
+    <t>Monteverdi</t>
+  </si>
+  <si>
+    <t>Moretti</t>
+  </si>
+  <si>
+    <t>Morris 1930</t>
+  </si>
+  <si>
+    <t>Moskvitch</t>
+  </si>
+  <si>
+    <t>Moskvitch 1940</t>
+  </si>
+  <si>
+    <t>Nash</t>
+  </si>
+  <si>
+    <t>Norton</t>
+  </si>
+  <si>
+    <t>NSU</t>
+  </si>
+  <si>
+    <t>Oldsmobile 1930</t>
+  </si>
+  <si>
+    <t>Osca</t>
+  </si>
+  <si>
+    <t>Packhard</t>
+  </si>
+  <si>
+    <t>Panoz</t>
+  </si>
+  <si>
+    <t>Pegaso</t>
+  </si>
+  <si>
+    <t>Pierce Arrow 1930</t>
+  </si>
+  <si>
+    <t>Pierce Arrow</t>
+  </si>
+  <si>
+    <t>Premier</t>
+  </si>
+  <si>
+    <t>Puch</t>
+  </si>
+  <si>
+    <t>Puma</t>
+  </si>
+  <si>
+    <t>Purvis</t>
+  </si>
+  <si>
+    <t>Quantum</t>
+  </si>
+  <si>
+    <t>Qvale</t>
+  </si>
+  <si>
+    <t>Reliant</t>
+  </si>
+  <si>
+    <t>Rene Bonnet 1930</t>
+  </si>
+  <si>
+    <t>Riley</t>
+  </si>
+  <si>
+    <t>Rosenberg</t>
+  </si>
+  <si>
+    <t>Saipa</t>
+  </si>
+  <si>
+    <t>Salmson 1930</t>
+  </si>
+  <si>
+    <t>Salmson</t>
+  </si>
+  <si>
+    <t>Scion</t>
+  </si>
+  <si>
+    <t>Seat 1980</t>
+  </si>
+  <si>
+    <t>Shelby 1960</t>
+  </si>
+  <si>
+    <t>Smart</t>
+  </si>
+  <si>
+    <t>Spectre</t>
+  </si>
+  <si>
+    <t>SsangYong 1980</t>
+  </si>
+  <si>
+    <t>SSC</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Sterling</t>
+  </si>
+  <si>
+    <t>Sterling 1930</t>
+  </si>
+  <si>
+    <t>Studebaker</t>
+  </si>
+  <si>
+    <t>Studebaler 1912</t>
+  </si>
+  <si>
+    <t>Stutz</t>
+  </si>
+  <si>
+    <t>Stutz 1940</t>
+  </si>
+  <si>
+    <t>Stutz 1960</t>
+  </si>
+  <si>
+    <t>Sunbeam</t>
+  </si>
+  <si>
+    <t>Sunbeam 1930</t>
+  </si>
+  <si>
+    <t>Talbot 1930</t>
+  </si>
+  <si>
+    <t>Tatra</t>
+  </si>
+  <si>
+    <t>Terrot</t>
+  </si>
+  <si>
+    <t>Terrot 1930</t>
+  </si>
+  <si>
+    <t>Tornado</t>
+  </si>
+  <si>
+    <t>Trabant</t>
+  </si>
+  <si>
+    <t>Trabant 1980</t>
+  </si>
+  <si>
+    <t>Voisin</t>
+  </si>
+  <si>
+    <t>Voxan</t>
+  </si>
+  <si>
+    <t>Wartburg</t>
+  </si>
+  <si>
+    <t>Western</t>
+  </si>
+  <si>
+    <t>Wolseley</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Citroën</t>
+  </si>
+  <si>
+    <t>Renault</t>
+  </si>
+  <si>
+    <t>Peugeot</t>
+  </si>
+  <si>
+    <t>Lancia</t>
+  </si>
+  <si>
+    <t>Opel</t>
+  </si>
+  <si>
+    <t>Alpine 1960</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>Skoda</t>
+  </si>
+  <si>
+    <t>Rover</t>
+  </si>
+  <si>
+    <t>Fiat</t>
+  </si>
+  <si>
+    <t>Saab</t>
+  </si>
+  <si>
+    <t>Seat</t>
+  </si>
+  <si>
+    <t>Matra 1960</t>
+  </si>
+  <si>
+    <t>Bizzarinni</t>
+  </si>
+  <si>
+    <t>Vaz</t>
+  </si>
+  <si>
+    <t>Rolls Royce</t>
+  </si>
+  <si>
+    <t>Lada</t>
+  </si>
+  <si>
+    <t>Zil</t>
+  </si>
+  <si>
+    <t>Melling</t>
+  </si>
+  <si>
+    <t>Hummer</t>
+  </si>
+  <si>
+    <t>Land Rover</t>
+  </si>
+  <si>
+    <t>Mini</t>
+  </si>
+  <si>
+    <t>Vauxhall</t>
+  </si>
+  <si>
+    <t>Acura</t>
+  </si>
+  <si>
+    <t>Dacia</t>
+  </si>
+  <si>
+    <t>Zastava 1980</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>Gaz</t>
+  </si>
+  <si>
+    <t>Ariel</t>
+  </si>
+  <si>
+    <t>Buick</t>
+  </si>
+  <si>
+    <t>Venturi</t>
+  </si>
+  <si>
+    <t>Daihatsu</t>
+  </si>
+  <si>
+    <t>Facel Vega</t>
+  </si>
+  <si>
+    <t>Simca</t>
+  </si>
+  <si>
+    <t>Abarth 1960</t>
+  </si>
+  <si>
+    <t>Alfa Romeo 1946</t>
+  </si>
+  <si>
+    <t>Alpina</t>
+  </si>
+  <si>
+    <t>AMC</t>
+  </si>
+  <si>
+    <t>Arash</t>
+  </si>
+  <si>
+    <t>Aston Martin 1947</t>
+  </si>
+  <si>
+    <t>Aston Martin 1984</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Austin Healey</t>
+  </si>
+  <si>
+    <t>Auto Union</t>
+  </si>
+  <si>
+    <t>Berliet</t>
+  </si>
+  <si>
+    <t>BFG</t>
+  </si>
+  <si>
+    <t>Bimota</t>
+  </si>
+  <si>
+    <t>Buell</t>
+  </si>
+  <si>
+    <t>Buell 1980</t>
+  </si>
+  <si>
+    <t>Buick 1990</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Internationnal</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>Chrysler 1950</t>
+  </si>
+  <si>
+    <t>Chrysler 1990</t>
+  </si>
+  <si>
+    <t>Citroen 1914</t>
+  </si>
+  <si>
+    <t>Citroen 1980</t>
+  </si>
+  <si>
+    <t>Claas</t>
+  </si>
+  <si>
+    <t>Cord</t>
+  </si>
+  <si>
+    <t>Dacia1930</t>
+  </si>
+  <si>
+    <t>Dacia1990</t>
+  </si>
+  <si>
+    <t>Vespa</t>
+  </si>
+  <si>
+    <t>Daewoo 1990</t>
+  </si>
+  <si>
+    <t>Daewoo</t>
+  </si>
+  <si>
+    <t>Daimler</t>
+  </si>
+  <si>
+    <t>Datsun 1930</t>
+  </si>
+  <si>
+    <t>Datsun</t>
+  </si>
+  <si>
+    <t>Dauer</t>
+  </si>
+  <si>
+    <t>Delage 1920</t>
+  </si>
+  <si>
+    <t>Delahaye</t>
+  </si>
+  <si>
+    <t>Detomaso</t>
+  </si>
+  <si>
+    <t>Dino</t>
+  </si>
+  <si>
+    <t>DMC</t>
+  </si>
+  <si>
+    <t>Eagle</t>
+  </si>
+  <si>
+    <t>Zastava</t>
+  </si>
+  <si>
+    <t>Farbio</t>
+  </si>
+  <si>
+    <t>Fendt</t>
+  </si>
+  <si>
+    <t>Fiat 1938</t>
+  </si>
+  <si>
+    <t>Fiat 1959</t>
+  </si>
+  <si>
+    <t>Fiat 1965</t>
+  </si>
+  <si>
+    <t>Fiat 1968</t>
+  </si>
+  <si>
+    <t>Fiat 1991</t>
+  </si>
+  <si>
+    <t>Fiat 1999</t>
+  </si>
+  <si>
+    <t>Flandria</t>
+  </si>
+  <si>
+    <t>Gemballa</t>
+  </si>
+  <si>
+    <t>Gillet</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>GMC</t>
+  </si>
+  <si>
+    <t>Gumpert</t>
+  </si>
+  <si>
+    <t>Harley Davidson</t>
+  </si>
+  <si>
+    <t>Heuliez</t>
+  </si>
+  <si>
+    <t>Hispano Suiza</t>
+  </si>
+  <si>
+    <t>Hommell</t>
+  </si>
+  <si>
+    <t>Honda Bike</t>
+  </si>
+  <si>
+    <t>Hyosung</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>Isuzu 1960</t>
+  </si>
+  <si>
+    <t>Isuzu</t>
+  </si>
+  <si>
+    <t>Italdesign</t>
+  </si>
+  <si>
+    <t>Iveco</t>
+  </si>
+  <si>
+    <t>Jeep</t>
+  </si>
+  <si>
+    <t>Jensen</t>
+  </si>
+  <si>
+    <t>John Deere</t>
+  </si>
+  <si>
+    <t>Kawasaki green</t>
+  </si>
+  <si>
+    <t>KIA</t>
+  </si>
+  <si>
+    <t>KTM</t>
+  </si>
+  <si>
+    <t>Zastava 1960</t>
+  </si>
+  <si>
+    <t>WSK</t>
+  </si>
+  <si>
+    <t>Lancia 1990</t>
+  </si>
+  <si>
+    <t>Landini</t>
+  </si>
+  <si>
+    <t>Laverda 1960</t>
+  </si>
+  <si>
+    <t>Laverda</t>
+  </si>
+  <si>
+    <t>Ligier</t>
+  </si>
+  <si>
+    <t>Ligier 1960</t>
+  </si>
+  <si>
+    <t>Lincoln</t>
+  </si>
+  <si>
+    <t>Marcos</t>
+  </si>
+  <si>
+    <t>Massey Fergusson</t>
+  </si>
+  <si>
+    <t>Matra 1970</t>
+  </si>
+  <si>
+    <t>Mazda 1968</t>
+  </si>
+  <si>
+    <t>Mazda 1991</t>
+  </si>
+  <si>
+    <t>Maybach</t>
+  </si>
+  <si>
+    <t>McCormick</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz 1950</t>
+  </si>
+  <si>
+    <t>Mercury</t>
+  </si>
+  <si>
+    <t>Morgan 1960</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>Morini</t>
+  </si>
+  <si>
+    <t>Morris</t>
+  </si>
+  <si>
+    <t>Mosler</t>
+  </si>
+  <si>
+    <t>Motobecane 1960</t>
+  </si>
+  <si>
+    <t>Motobecane</t>
+  </si>
+  <si>
+    <t>Moto Guzzi</t>
+  </si>
+  <si>
+    <t>New Holland</t>
+  </si>
+  <si>
+    <t>Nissan 1970</t>
+  </si>
+  <si>
+    <t>Oldsmobile</t>
+  </si>
+  <si>
+    <t>Opel 1937</t>
+  </si>
+  <si>
+    <t>Opel 1947</t>
+  </si>
+  <si>
+    <t>Opel 1954</t>
+  </si>
+  <si>
+    <t>Opel 1964</t>
+  </si>
+  <si>
+    <t>Panhard</t>
+  </si>
+  <si>
+    <t>Peugeot 1936</t>
+  </si>
+  <si>
+    <t>Peugeot 1950</t>
+  </si>
+  <si>
+    <t>Peugeot 1960</t>
+  </si>
+  <si>
+    <t>Peugeot 1965</t>
+  </si>
+  <si>
+    <t>Peugeot 1980</t>
+  </si>
+  <si>
+    <t>Peugeot 1995</t>
+  </si>
+  <si>
+    <t>Proton</t>
+  </si>
+  <si>
+    <t>Renault 1946</t>
+  </si>
+  <si>
+    <t>Renault 1972</t>
+  </si>
+  <si>
+    <t>Renault 1992</t>
+  </si>
+  <si>
+    <t>Rennet Bonnet</t>
+  </si>
+  <si>
+    <t>Royal Enfield 1930</t>
+  </si>
+  <si>
+    <t>Royal Enfield</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>Sbarro</t>
+  </si>
+  <si>
+    <t>Scania</t>
+  </si>
+  <si>
+    <t>Shuanghuan</t>
+  </si>
+  <si>
+    <t>Someca</t>
+  </si>
+  <si>
+    <t>Ssangyong</t>
+  </si>
+  <si>
+    <t>Talbot</t>
+  </si>
+  <si>
+    <t>Tata</t>
+  </si>
+  <si>
+    <t>Zaz</t>
+  </si>
+  <si>
+    <t>Zaz 1961</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Plymouth 1940</t>
+  </si>
+  <si>
+    <t>Porsche</t>
+  </si>
+  <si>
+    <t>Bentley</t>
+  </si>
+  <si>
+    <t>Bizzarinni 1960</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>Infiniti</t>
+  </si>
+  <si>
+    <t>Bugatti</t>
+  </si>
+  <si>
+    <t>Mitsubishi</t>
+  </si>
+  <si>
+    <t>Aprilia</t>
+  </si>
+  <si>
+    <t>Benelli</t>
+  </si>
+  <si>
+    <t>Yamaha blue</t>
+  </si>
+  <si>
+    <t>yamaha red</t>
+  </si>
+  <si>
+    <t>Subaru</t>
+  </si>
+  <si>
+    <t>Hennessey Performance</t>
+  </si>
+  <si>
+    <t>Radical</t>
+  </si>
+  <si>
+    <t>Rossion</t>
+  </si>
+  <si>
+    <t>Triumph 1960</t>
+  </si>
+  <si>
+    <t>Vauxhall 1930</t>
+  </si>
+  <si>
+    <t>Vauxhall 1970</t>
+  </si>
+  <si>
+    <t>Vauxhall 2000</t>
+  </si>
+  <si>
+    <t>Zaz 1970</t>
+  </si>
+  <si>
+    <t>Zaz 1980</t>
+  </si>
+  <si>
+    <t>Abarth</t>
+  </si>
+  <si>
+    <t>AMCA</t>
+  </si>
+  <si>
+    <t>Arista</t>
+  </si>
+  <si>
+    <t>Aixam</t>
+  </si>
+  <si>
+    <t>Allard</t>
+  </si>
+  <si>
+    <t>Alpine</t>
+  </si>
+  <si>
+    <t>Alpine 1970</t>
+  </si>
+  <si>
+    <t>Alvis</t>
+  </si>
+  <si>
+    <t>AMC 1950</t>
+  </si>
+  <si>
+    <t>Amilcar</t>
+  </si>
+  <si>
+    <t>Amilcar 1930</t>
+  </si>
+  <si>
+    <t>Amilcar 1950</t>
+  </si>
+  <si>
+    <t>ARO</t>
+  </si>
+  <si>
+    <t>ASA</t>
+  </si>
+  <si>
+    <t>MV Agusta</t>
+  </si>
+  <si>
+    <t>Aston Martin 1920</t>
+  </si>
+  <si>
+    <t>Auburn</t>
+  </si>
+  <si>
+    <t>Austin Healey 1930</t>
+  </si>
+  <si>
+    <t>Austin Rover</t>
+  </si>
+  <si>
+    <t>Autobianchi</t>
+  </si>
+  <si>
+    <t>Avanti</t>
+  </si>
+  <si>
+    <t>Bajaj</t>
+  </si>
+  <si>
+    <t>Ballot</t>
+  </si>
+  <si>
+    <t>Bertone</t>
+  </si>
+  <si>
+    <t>Bertone 1930</t>
+  </si>
+  <si>
+    <t>Bitter</t>
+  </si>
+  <si>
+    <t>Bogward</t>
+  </si>
+  <si>
+    <t>Bristol 1930</t>
+  </si>
+  <si>
+    <t>Bristol</t>
+  </si>
+  <si>
+    <t>BSA</t>
+  </si>
+  <si>
+    <t>Bultaco</t>
+  </si>
+  <si>
+    <t>Caterham</t>
+  </si>
+  <si>
+    <t>Chevrolet 1970</t>
+  </si>
+  <si>
+    <t>Citroen 1960</t>
+  </si>
+  <si>
+    <t>Cizeta</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>Corre La Licorne</t>
+  </si>
+  <si>
+    <t>Coste</t>
+  </si>
+  <si>
+    <t>DAF</t>
+  </si>
+  <si>
+    <t>DAF 1950</t>
+  </si>
+  <si>
+    <t>DAF 1960</t>
+  </si>
+  <si>
+    <t>Daimler 1960</t>
+  </si>
+  <si>
+    <t>Delage</t>
+  </si>
+  <si>
+    <t>DeSoto</t>
+  </si>
+  <si>
+    <t>DKW</t>
+  </si>
+  <si>
+    <t>Donkervoort</t>
+  </si>
+  <si>
+    <t>Ducati 1970</t>
+  </si>
+  <si>
+    <t>Duesenberg 8</t>
+  </si>
+  <si>
+    <t>Duesenberg 12</t>
+  </si>
+  <si>
+    <t>Eagle 1960</t>
+  </si>
+  <si>
+    <t>Edsel</t>
+  </si>
+  <si>
+    <t>Elva</t>
+  </si>
+  <si>
+    <t>Ferrari 1950</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>Geely</t>
+  </si>
+  <si>
+    <t>Geo</t>
+  </si>
+  <si>
+    <t>Ginetta</t>
+  </si>
+  <si>
+    <t>Gordini</t>
+  </si>
+  <si>
+    <t>Hillman</t>
+  </si>
+  <si>
+    <t>Hindustan</t>
+  </si>
+  <si>
+    <t>Hodaka</t>
+  </si>
+  <si>
+    <t>Hudson</t>
+  </si>
+  <si>
+    <t>Hudson 1930</t>
+  </si>
+  <si>
+    <t>Iso</t>
+  </si>
+  <si>
+    <t>Jeep 1980</t>
+  </si>
+  <si>
+    <t>Josse</t>
+  </si>
+  <si>
+    <t>Kaiser</t>
+  </si>
+  <si>
+    <t>Kaiser 1930</t>
+  </si>
+  <si>
+    <t>Lagonda</t>
+  </si>
+  <si>
+    <t>Lightning</t>
+  </si>
+  <si>
+    <t>Lincoln 1930</t>
+  </si>
+  <si>
+    <t>Lola</t>
+  </si>
+  <si>
+    <t>Lotec</t>
+  </si>
+  <si>
+    <t>Luaz</t>
+  </si>
+  <si>
+    <t>Matra</t>
+  </si>
+  <si>
+    <t>MCV</t>
+  </si>
+  <si>
+    <t>Jaguar</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>RUF</t>
+  </si>
+  <si>
+    <t>B. Engineering</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>TVR</t>
+  </si>
+  <si>
+    <t>Suzuki</t>
+  </si>
+  <si>
+    <t>Ascari</t>
+  </si>
+  <si>
+    <t>Alfa Romeo</t>
+  </si>
+  <si>
+    <t>Kawasaki</t>
+  </si>
+  <si>
+    <t>Farboud</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Audi</t>
+  </si>
+  <si>
+    <t>Spyker</t>
+  </si>
+  <si>
+    <t>Koenigsegg</t>
+  </si>
+  <si>
+    <t>Plymouth</t>
+  </si>
+  <si>
+    <t>Generic Car</t>
+  </si>
+  <si>
+    <t>Pontiac</t>
+  </si>
+  <si>
+    <t>Mazda</t>
+  </si>
+  <si>
+    <t>Dodge</t>
+  </si>
+  <si>
+    <t>Noble</t>
+  </si>
+  <si>
+    <t>Lamborghini</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz</t>
+  </si>
+  <si>
+    <t>Aston Martin</t>
+  </si>
+  <si>
+    <t>Maserati</t>
+  </si>
+  <si>
+    <t>Caterham 1990</t>
+  </si>
+  <si>
+    <t>Ducati</t>
+  </si>
+  <si>
+    <t>Lotus</t>
+  </si>
+  <si>
+    <t>Lexus</t>
+  </si>
+  <si>
+    <t>Chrysler</t>
+  </si>
+  <si>
+    <t>Chevrolet</t>
+  </si>
+  <si>
+    <t>Nismo</t>
+  </si>
+  <si>
+    <t>Pagani</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>Saleen</t>
+  </si>
+  <si>
+    <t>Saturn</t>
+  </si>
+  <si>
+    <t>Shelby</t>
+  </si>
+  <si>
+    <t>Holden</t>
+  </si>
+  <si>
+    <t>Brabus</t>
+  </si>
+  <si>
+    <t>Cadillac</t>
+  </si>
+  <si>
+    <t>TRAFFIC</t>
+  </si>
+  <si>
+    <t>Triumph</t>
+  </si>
+  <si>
+    <t>Ferrari</t>
+  </si>
+  <si>
+    <t>McLaren</t>
+  </si>
+  <si>
+    <t>Hennessey</t>
+  </si>
+  <si>
+    <t>Wiesmann</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -7959,8 +9093,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7971,6 +9116,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
         <bgColor rgb="FFD0D7E5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -8013,13 +9164,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -8028,11 +9180,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -8042,7 +9194,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -8052,9 +9204,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Texte explicatif" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -19880,7 +21043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B619"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -24852,4 +26015,3045 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B377"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>2886</v>
+      </c>
+      <c r="B2" s="19">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>2733</v>
+      </c>
+      <c r="B3" s="19">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B4" s="19">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>2722</v>
+      </c>
+      <c r="B5" s="19">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>2889</v>
+      </c>
+      <c r="B6" s="19">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>2971</v>
+      </c>
+      <c r="B7" s="19">
+        <v>72825</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>2734</v>
+      </c>
+      <c r="B8" s="19">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>2890</v>
+      </c>
+      <c r="B9" s="19">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>2735</v>
+      </c>
+      <c r="B10" s="19">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>2891</v>
+      </c>
+      <c r="B11" s="19">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>2704</v>
+      </c>
+      <c r="B12" s="19">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>2892</v>
+      </c>
+      <c r="B13" s="19">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>2893</v>
+      </c>
+      <c r="B14" s="19">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>2736</v>
+      </c>
+      <c r="B15" s="19">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>2894</v>
+      </c>
+      <c r="B16" s="19">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>2887</v>
+      </c>
+      <c r="B17" s="19">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>2895</v>
+      </c>
+      <c r="B18" s="19">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>2896</v>
+      </c>
+      <c r="B19" s="19">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>2897</v>
+      </c>
+      <c r="B20" s="19">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>2872</v>
+      </c>
+      <c r="B21" s="19">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>2737</v>
+      </c>
+      <c r="B22" s="19">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>2727</v>
+      </c>
+      <c r="B23" s="19">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>2888</v>
+      </c>
+      <c r="B24" s="19">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>2898</v>
+      </c>
+      <c r="B25" s="19">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>2899</v>
+      </c>
+      <c r="B26" s="19">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>2970</v>
+      </c>
+      <c r="B27" s="19">
+        <v>72595</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>2986</v>
+      </c>
+      <c r="B28" s="19">
+        <v>868295</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>2901</v>
+      </c>
+      <c r="B29" s="19">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>2738</v>
+      </c>
+      <c r="B30" s="19">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>2739</v>
+      </c>
+      <c r="B31" s="19">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>2902</v>
+      </c>
+      <c r="B32" s="19">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>2975</v>
+      </c>
+      <c r="B33" s="19">
+        <v>80715</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>2740</v>
+      </c>
+      <c r="B34" s="19">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B35" s="19">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>2903</v>
+      </c>
+      <c r="B36" s="19">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>2904</v>
+      </c>
+      <c r="B37" s="19">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>2742</v>
+      </c>
+      <c r="B38" s="19">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
+        <v>2905</v>
+      </c>
+      <c r="B39" s="19">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
+        <v>2906</v>
+      </c>
+      <c r="B40" s="19">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>2966</v>
+      </c>
+      <c r="B41" s="19">
+        <v>8649</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>2907</v>
+      </c>
+      <c r="B42" s="19">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>2908</v>
+      </c>
+      <c r="B43" s="19">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
+        <v>2873</v>
+      </c>
+      <c r="B44" s="19">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>2866</v>
+      </c>
+      <c r="B45" s="19">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
+        <v>2743</v>
+      </c>
+      <c r="B46" s="19">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
+        <v>2909</v>
+      </c>
+      <c r="B47" s="19">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
+        <v>2910</v>
+      </c>
+      <c r="B48" s="19">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
+        <v>2744</v>
+      </c>
+      <c r="B49" s="19">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
+        <v>2745</v>
+      </c>
+      <c r="B50" s="19">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>2911</v>
+      </c>
+      <c r="B51" s="19">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
+        <v>2712</v>
+      </c>
+      <c r="B52" s="19">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
+        <v>2867</v>
+      </c>
+      <c r="B53" s="19">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="18" t="s">
+        <v>2868</v>
+      </c>
+      <c r="B54" s="19">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>2912</v>
+      </c>
+      <c r="B55" s="19">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="18" t="s">
+        <v>3001</v>
+      </c>
+      <c r="B56" s="19">
+        <v>12778906</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
+        <v>2914</v>
+      </c>
+      <c r="B57" s="19">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="18" t="s">
+        <v>2913</v>
+      </c>
+      <c r="B58" s="19">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>2915</v>
+      </c>
+      <c r="B59" s="19">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>2746</v>
+      </c>
+      <c r="B60" s="19">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
+        <v>2747</v>
+      </c>
+      <c r="B61" s="19">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
+        <v>2870</v>
+      </c>
+      <c r="B62" s="19">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
+        <v>2728</v>
+      </c>
+      <c r="B63" s="19">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="18" t="s">
+        <v>2748</v>
+      </c>
+      <c r="B64" s="19">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="18" t="s">
+        <v>2916</v>
+      </c>
+      <c r="B65" s="19">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="18" t="s">
+        <v>3002</v>
+      </c>
+      <c r="B66" s="19">
+        <v>74340517</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="18" t="s">
+        <v>2749</v>
+      </c>
+      <c r="B67" s="19">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="18" t="s">
+        <v>2751</v>
+      </c>
+      <c r="B68" s="19">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="18" t="s">
+        <v>2917</v>
+      </c>
+      <c r="B69" s="19">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="18" t="s">
+        <v>2988</v>
+      </c>
+      <c r="B70" s="19">
+        <v>898117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="18" t="s">
+        <v>2993</v>
+      </c>
+      <c r="B71" s="19">
+        <v>983687</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="18" t="s">
+        <v>2918</v>
+      </c>
+      <c r="B72" s="19">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="18" t="s">
+        <v>2992</v>
+      </c>
+      <c r="B73" s="19">
+        <v>927987</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="18" t="s">
+        <v>2752</v>
+      </c>
+      <c r="B74" s="19">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="18" t="s">
+        <v>2753</v>
+      </c>
+      <c r="B75" s="19">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="18" t="s">
+        <v>2699</v>
+      </c>
+      <c r="B76" s="19">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
+        <v>2754</v>
+      </c>
+      <c r="B77" s="19">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
+        <v>2919</v>
+      </c>
+      <c r="B78" s="19">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
+        <v>2755</v>
+      </c>
+      <c r="B79" s="19">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="18" t="s">
+        <v>2920</v>
+      </c>
+      <c r="B80" s="19">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="18" t="s">
+        <v>2756</v>
+      </c>
+      <c r="B81" s="19">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="18" t="s">
+        <v>2921</v>
+      </c>
+      <c r="B82" s="19">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="18" t="s">
+        <v>2757</v>
+      </c>
+      <c r="B83" s="19">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="18" t="s">
+        <v>2922</v>
+      </c>
+      <c r="B84" s="19">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
+        <v>2923</v>
+      </c>
+      <c r="B85" s="19">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="18" t="s">
+        <v>2723</v>
+      </c>
+      <c r="B86" s="19">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
+        <v>2758</v>
+      </c>
+      <c r="B87" s="19">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>2759</v>
+      </c>
+      <c r="B88" s="19">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
+        <v>2762</v>
+      </c>
+      <c r="B89" s="19">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="18" t="s">
+        <v>2761</v>
+      </c>
+      <c r="B90" s="19">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="18" t="s">
+        <v>2924</v>
+      </c>
+      <c r="B91" s="19">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="18" t="s">
+        <v>2925</v>
+      </c>
+      <c r="B92" s="19">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="18" t="s">
+        <v>2926</v>
+      </c>
+      <c r="B93" s="19">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="18" t="s">
+        <v>2730</v>
+      </c>
+      <c r="B94" s="19">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="18" t="s">
+        <v>2763</v>
+      </c>
+      <c r="B95" s="19">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="18" t="s">
+        <v>2927</v>
+      </c>
+      <c r="B96" s="19">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="18" t="s">
+        <v>2765</v>
+      </c>
+      <c r="B97" s="19">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="18" t="s">
+        <v>2764</v>
+      </c>
+      <c r="B98" s="19">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="18" t="s">
+        <v>2766</v>
+      </c>
+      <c r="B99" s="19">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="18" t="s">
+        <v>2928</v>
+      </c>
+      <c r="B100" s="19">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="18" t="s">
+        <v>2767</v>
+      </c>
+      <c r="B101" s="19">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="18" t="s">
+        <v>2768</v>
+      </c>
+      <c r="B102" s="19">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="18" t="s">
+        <v>2929</v>
+      </c>
+      <c r="B103" s="19">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="18" t="s">
+        <v>2769</v>
+      </c>
+      <c r="B104" s="19">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="18" t="s">
+        <v>2770</v>
+      </c>
+      <c r="B105" s="19">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="18" t="s">
+        <v>2930</v>
+      </c>
+      <c r="B106" s="19">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="18" t="s">
+        <v>2771</v>
+      </c>
+      <c r="B107" s="19">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="18" t="s">
+        <v>2982</v>
+      </c>
+      <c r="B108" s="19">
+        <v>768658</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="18" t="s">
+        <v>2931</v>
+      </c>
+      <c r="B109" s="19">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="18" t="s">
+        <v>2989</v>
+      </c>
+      <c r="B110" s="19">
+        <v>912618</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="18" t="s">
+        <v>2932</v>
+      </c>
+      <c r="B111" s="19">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="18" t="s">
+        <v>2934</v>
+      </c>
+      <c r="B112" s="19">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="18" t="s">
+        <v>2933</v>
+      </c>
+      <c r="B113" s="19">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="18" t="s">
+        <v>2772</v>
+      </c>
+      <c r="B114" s="19">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="18" t="s">
+        <v>2935</v>
+      </c>
+      <c r="B115" s="19">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="18" t="s">
+        <v>2936</v>
+      </c>
+      <c r="B116" s="19">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="18" t="s">
+        <v>2937</v>
+      </c>
+      <c r="B117" s="19">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="18" t="s">
+        <v>2731</v>
+      </c>
+      <c r="B118" s="19">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="18" t="s">
+        <v>2774</v>
+      </c>
+      <c r="B119" s="19">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="18" t="s">
+        <v>2973</v>
+      </c>
+      <c r="B120" s="19">
+        <v>74920</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="18" t="s">
+        <v>2775</v>
+      </c>
+      <c r="B121" s="19">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="18" t="s">
+        <v>3005</v>
+      </c>
+      <c r="B122" s="19">
+        <v>81940960</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="18" t="s">
+        <v>2938</v>
+      </c>
+      <c r="B123" s="19">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="18" t="s">
+        <v>2708</v>
+      </c>
+      <c r="B124" s="19">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="18" t="s">
+        <v>2776</v>
+      </c>
+      <c r="B125" s="19">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="18" t="s">
+        <v>2777</v>
+      </c>
+      <c r="B126" s="19">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="18" t="s">
+        <v>2778</v>
+      </c>
+      <c r="B127" s="19">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="18" t="s">
+        <v>2779</v>
+      </c>
+      <c r="B128" s="19">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="18" t="s">
+        <v>2780</v>
+      </c>
+      <c r="B129" s="19">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="18" t="s">
+        <v>2781</v>
+      </c>
+      <c r="B130" s="19">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="18" t="s">
+        <v>2782</v>
+      </c>
+      <c r="B131" s="19">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="18" t="s">
+        <v>2939</v>
+      </c>
+      <c r="B132" s="19">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="18" t="s">
+        <v>2974</v>
+      </c>
+      <c r="B133" s="19">
+        <v>77060</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="18" t="s">
+        <v>2726</v>
+      </c>
+      <c r="B134" s="19">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="18" t="s">
+        <v>2726</v>
+      </c>
+      <c r="B135" s="19">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="18" t="s">
+        <v>2940</v>
+      </c>
+      <c r="B136" s="19">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="18" t="s">
+        <v>2783</v>
+      </c>
+      <c r="B137" s="19">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="18" t="s">
+        <v>2979</v>
+      </c>
+      <c r="B138" s="19">
+        <v>91197</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="18" t="s">
+        <v>2941</v>
+      </c>
+      <c r="B139" s="19">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="18" t="s">
+        <v>2784</v>
+      </c>
+      <c r="B140" s="19">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="18" t="s">
+        <v>2942</v>
+      </c>
+      <c r="B141" s="19">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="18" t="s">
+        <v>2785</v>
+      </c>
+      <c r="B142" s="19">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="18" t="s">
+        <v>2786</v>
+      </c>
+      <c r="B143" s="19">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="18" t="s">
+        <v>2943</v>
+      </c>
+      <c r="B144" s="19">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="18" t="s">
+        <v>2787</v>
+      </c>
+      <c r="B145" s="19">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="18" t="s">
+        <v>2788</v>
+      </c>
+      <c r="B146" s="19">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="18" t="s">
+        <v>3007</v>
+      </c>
+      <c r="B147" s="19">
+        <v>1137632324</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="18" t="s">
+        <v>2877</v>
+      </c>
+      <c r="B148" s="19">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="18" t="s">
+        <v>2789</v>
+      </c>
+      <c r="B149" s="19">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="18" t="s">
+        <v>2944</v>
+      </c>
+      <c r="B150" s="19">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="18" t="s">
+        <v>2945</v>
+      </c>
+      <c r="B151" s="19">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="18" t="s">
+        <v>2790</v>
+      </c>
+      <c r="B152" s="19">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="18" t="s">
+        <v>2946</v>
+      </c>
+      <c r="B153" s="19">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="18" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B154" s="19">
+        <v>12121982</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="18" t="s">
+        <v>2791</v>
+      </c>
+      <c r="B155" s="19">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="18" t="s">
+        <v>2964</v>
+      </c>
+      <c r="B156" s="19">
+        <v>7853</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="18" t="s">
+        <v>2792</v>
+      </c>
+      <c r="B157" s="19">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="18" t="s">
+        <v>2947</v>
+      </c>
+      <c r="B158" s="19">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="18" t="s">
+        <v>2948</v>
+      </c>
+      <c r="B159" s="19">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="18" t="s">
+        <v>2718</v>
+      </c>
+      <c r="B160" s="19">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="18" t="s">
+        <v>2793</v>
+      </c>
+      <c r="B161" s="19">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="18" t="s">
+        <v>2794</v>
+      </c>
+      <c r="B162" s="19">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="18" t="s">
+        <v>2869</v>
+      </c>
+      <c r="B163" s="19">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="18" t="s">
+        <v>2750</v>
+      </c>
+      <c r="B164" s="19">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="18" t="s">
+        <v>2949</v>
+      </c>
+      <c r="B165" s="19">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="18" t="s">
+        <v>2796</v>
+      </c>
+      <c r="B166" s="19">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="18" t="s">
+        <v>2795</v>
+      </c>
+      <c r="B167" s="19">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="18" t="s">
+        <v>2797</v>
+      </c>
+      <c r="B168" s="19">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="18" t="s">
+        <v>2798</v>
+      </c>
+      <c r="B169" s="19">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="18" t="s">
+        <v>2962</v>
+      </c>
+      <c r="B170" s="19">
+        <v>7824</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="18" t="s">
+        <v>2799</v>
+      </c>
+      <c r="B171" s="19">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="18" t="s">
+        <v>2950</v>
+      </c>
+      <c r="B172" s="19">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="18" t="s">
+        <v>2800</v>
+      </c>
+      <c r="B173" s="19">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="18" t="s">
+        <v>2801</v>
+      </c>
+      <c r="B174" s="19">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="18" t="s">
+        <v>2951</v>
+      </c>
+      <c r="B175" s="19">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="18" t="s">
+        <v>2952</v>
+      </c>
+      <c r="B176" s="19">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="18" t="s">
+        <v>2953</v>
+      </c>
+      <c r="B177" s="19">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="18" t="s">
+        <v>2972</v>
+      </c>
+      <c r="B178" s="19">
+        <v>74425</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="18" t="s">
+        <v>2802</v>
+      </c>
+      <c r="B179" s="19">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="18" t="s">
+        <v>2803</v>
+      </c>
+      <c r="B180" s="19">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="18" t="s">
+        <v>2977</v>
+      </c>
+      <c r="B181" s="19">
+        <v>85765</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="18" t="s">
+        <v>2804</v>
+      </c>
+      <c r="B182" s="19">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="18" t="s">
+        <v>2715</v>
+      </c>
+      <c r="B183" s="19">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="18" t="s">
+        <v>2954</v>
+      </c>
+      <c r="B184" s="19">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="18" t="s">
+        <v>2984</v>
+      </c>
+      <c r="B185" s="19">
+        <v>864426</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="18" t="s">
+        <v>2702</v>
+      </c>
+      <c r="B186" s="19">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="18" t="s">
+        <v>2807</v>
+      </c>
+      <c r="B187" s="19">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="18" t="s">
+        <v>2719</v>
+      </c>
+      <c r="B188" s="19">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="18" t="s">
+        <v>2808</v>
+      </c>
+      <c r="B189" s="19">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="18" t="s">
+        <v>2810</v>
+      </c>
+      <c r="B190" s="19">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="18" t="s">
+        <v>2809</v>
+      </c>
+      <c r="B191" s="19">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="18" t="s">
+        <v>2991</v>
+      </c>
+      <c r="B192" s="19">
+        <v>924566</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="18" t="s">
+        <v>2955</v>
+      </c>
+      <c r="B193" s="19">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="18" t="s">
+        <v>2811</v>
+      </c>
+      <c r="B194" s="19">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="18" t="s">
+        <v>2812</v>
+      </c>
+      <c r="B195" s="19">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="18" t="s">
+        <v>2813</v>
+      </c>
+      <c r="B196" s="19">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="18" t="s">
+        <v>2956</v>
+      </c>
+      <c r="B197" s="19">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="18" t="s">
+        <v>2957</v>
+      </c>
+      <c r="B198" s="19">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="18" t="s">
+        <v>2958</v>
+      </c>
+      <c r="B199" s="19">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="18" t="s">
+        <v>2990</v>
+      </c>
+      <c r="B200" s="19">
+        <v>924266</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="18" t="s">
+        <v>2959</v>
+      </c>
+      <c r="B201" s="19">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="18" t="s">
+        <v>2814</v>
+      </c>
+      <c r="B202" s="19">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="18" t="s">
+        <v>2987</v>
+      </c>
+      <c r="B203" s="19">
+        <v>898027</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="18" t="s">
+        <v>2815</v>
+      </c>
+      <c r="B204" s="19">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="18" t="s">
+        <v>2960</v>
+      </c>
+      <c r="B205" s="19">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="18" t="s">
+        <v>2711</v>
+      </c>
+      <c r="B206" s="19">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="18" t="s">
+        <v>2816</v>
+      </c>
+      <c r="B207" s="19">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="18" t="s">
+        <v>2819</v>
+      </c>
+      <c r="B208" s="19">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="18" t="s">
+        <v>2981</v>
+      </c>
+      <c r="B209" s="19">
+        <v>727727</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="18" t="s">
+        <v>2817</v>
+      </c>
+      <c r="B210" s="19">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="18" t="s">
+        <v>2818</v>
+      </c>
+      <c r="B211" s="19">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="18" t="s">
+        <v>2820</v>
+      </c>
+      <c r="B212" s="19">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="18" t="s">
+        <v>3006</v>
+      </c>
+      <c r="B213" s="19">
+        <v>85793347</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="18" t="s">
+        <v>2961</v>
+      </c>
+      <c r="B214" s="19">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="18" t="s">
+        <v>2634</v>
+      </c>
+      <c r="B215" s="19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="18" t="s">
+        <v>2717</v>
+      </c>
+      <c r="B216" s="19">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="18" t="s">
+        <v>2985</v>
+      </c>
+      <c r="B217" s="19">
+        <v>865967</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="18" t="s">
+        <v>2635</v>
+      </c>
+      <c r="B218" s="19">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="18" t="s">
+        <v>2636</v>
+      </c>
+      <c r="B219" s="19">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="18" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B220" s="19">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="18" t="s">
+        <v>2822</v>
+      </c>
+      <c r="B221" s="19">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" s="18" t="s">
+        <v>2823</v>
+      </c>
+      <c r="B222" s="19">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="18" t="s">
+        <v>2638</v>
+      </c>
+      <c r="B223" s="19">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="18" t="s">
+        <v>2639</v>
+      </c>
+      <c r="B224" s="19">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" s="18" t="s">
+        <v>2720</v>
+      </c>
+      <c r="B225" s="19">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" s="18" t="s">
+        <v>2871</v>
+      </c>
+      <c r="B226" s="19">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" s="18" t="s">
+        <v>2640</v>
+      </c>
+      <c r="B227" s="19">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" s="18" t="s">
+        <v>2641</v>
+      </c>
+      <c r="B228" s="19">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="18" t="s">
+        <v>2642</v>
+      </c>
+      <c r="B229" s="19">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" s="18" t="s">
+        <v>2825</v>
+      </c>
+      <c r="B230" s="19">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" s="18" t="s">
+        <v>2824</v>
+      </c>
+      <c r="B231" s="19">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" s="18" t="s">
+        <v>2826</v>
+      </c>
+      <c r="B232" s="19">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" s="18" t="s">
+        <v>2827</v>
+      </c>
+      <c r="B233" s="19">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" s="18" t="s">
+        <v>2643</v>
+      </c>
+      <c r="B234" s="19">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="18" t="s">
+        <v>2644</v>
+      </c>
+      <c r="B235" s="19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="18" t="s">
+        <v>2645</v>
+      </c>
+      <c r="B236" s="19">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" s="18" t="s">
+        <v>2828</v>
+      </c>
+      <c r="B237" s="19">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" s="18" t="s">
+        <v>2831</v>
+      </c>
+      <c r="B238" s="19">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" s="18" t="s">
+        <v>2830</v>
+      </c>
+      <c r="B239" s="19">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" s="18" t="s">
+        <v>2829</v>
+      </c>
+      <c r="B240" s="19">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="18" t="s">
+        <v>2900</v>
+      </c>
+      <c r="B241" s="19">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" s="18" t="s">
+        <v>2646</v>
+      </c>
+      <c r="B242" s="19">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" s="18" t="s">
+        <v>2832</v>
+      </c>
+      <c r="B243" s="19">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" s="18" t="s">
+        <v>2994</v>
+      </c>
+      <c r="B244" s="19">
+        <v>1231628</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" s="18" t="s">
+        <v>2996</v>
+      </c>
+      <c r="B245" s="19">
+        <v>8542108</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" s="18" t="s">
+        <v>2833</v>
+      </c>
+      <c r="B246" s="19">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="18" t="s">
+        <v>2983</v>
+      </c>
+      <c r="B247" s="19">
+        <v>773468</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="18" t="s">
+        <v>2647</v>
+      </c>
+      <c r="B248" s="19">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" s="18" t="s">
+        <v>2648</v>
+      </c>
+      <c r="B249" s="19">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="18" t="s">
+        <v>2834</v>
+      </c>
+      <c r="B250" s="19">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="18" t="s">
+        <v>2649</v>
+      </c>
+      <c r="B251" s="19">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="18" t="s">
+        <v>2703</v>
+      </c>
+      <c r="B252" s="19">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="18" t="s">
+        <v>2835</v>
+      </c>
+      <c r="B253" s="19">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" s="18" t="s">
+        <v>2836</v>
+      </c>
+      <c r="B254" s="19">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" s="18" t="s">
+        <v>2837</v>
+      </c>
+      <c r="B255" s="19">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" s="18" t="s">
+        <v>2838</v>
+      </c>
+      <c r="B256" s="19">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" s="18" t="s">
+        <v>2650</v>
+      </c>
+      <c r="B257" s="19">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" s="18" t="s">
+        <v>2651</v>
+      </c>
+      <c r="B258" s="19">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" s="18" t="s">
+        <v>2995</v>
+      </c>
+      <c r="B259" s="19">
+        <v>8152830</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" s="18" t="s">
+        <v>2839</v>
+      </c>
+      <c r="B260" s="19">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="18" t="s">
+        <v>2652</v>
+      </c>
+      <c r="B261" s="19">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" s="18" t="s">
+        <v>2653</v>
+      </c>
+      <c r="B262" s="19">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="18" t="s">
+        <v>2701</v>
+      </c>
+      <c r="B263" s="19">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="18" t="s">
+        <v>2840</v>
+      </c>
+      <c r="B264" s="19">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" s="18" t="s">
+        <v>2841</v>
+      </c>
+      <c r="B265" s="19">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" s="18" t="s">
+        <v>2842</v>
+      </c>
+      <c r="B266" s="19">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" s="18" t="s">
+        <v>2843</v>
+      </c>
+      <c r="B267" s="19">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" s="18" t="s">
+        <v>2844</v>
+      </c>
+      <c r="B268" s="19">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" s="18" t="s">
+        <v>2845</v>
+      </c>
+      <c r="B269" s="19">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" s="18" t="s">
+        <v>2655</v>
+      </c>
+      <c r="B270" s="19">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" s="18" t="s">
+        <v>2654</v>
+      </c>
+      <c r="B271" s="19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" s="18" t="s">
+        <v>2978</v>
+      </c>
+      <c r="B272" s="19">
+        <v>86740</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" s="18" t="s">
+        <v>2864</v>
+      </c>
+      <c r="B273" s="19">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" s="18" t="s">
+        <v>2980</v>
+      </c>
+      <c r="B274" s="19">
+        <v>92670</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" s="18" t="s">
+        <v>2865</v>
+      </c>
+      <c r="B275" s="19">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" s="18" t="s">
+        <v>2656</v>
+      </c>
+      <c r="B276" s="19">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" s="18" t="s">
+        <v>2846</v>
+      </c>
+      <c r="B277" s="19">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" s="18" t="s">
+        <v>2657</v>
+      </c>
+      <c r="B278" s="19">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="18" t="s">
+        <v>2658</v>
+      </c>
+      <c r="B279" s="19">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="18" t="s">
+        <v>2659</v>
+      </c>
+      <c r="B280" s="19">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="18" t="s">
+        <v>2660</v>
+      </c>
+      <c r="B281" s="19">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="18" t="s">
+        <v>2661</v>
+      </c>
+      <c r="B282" s="19">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" s="18" t="s">
+        <v>2878</v>
+      </c>
+      <c r="B283" s="19">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" s="18" t="s">
+        <v>2662</v>
+      </c>
+      <c r="B284" s="19">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="18" t="s">
+        <v>2700</v>
+      </c>
+      <c r="B285" s="19">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" s="18" t="s">
+        <v>2847</v>
+      </c>
+      <c r="B286" s="19">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" s="18" t="s">
+        <v>2848</v>
+      </c>
+      <c r="B287" s="19">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" s="18" t="s">
+        <v>2849</v>
+      </c>
+      <c r="B288" s="19">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" s="18" t="s">
+        <v>2663</v>
+      </c>
+      <c r="B289" s="19">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" s="18" t="s">
+        <v>2850</v>
+      </c>
+      <c r="B290" s="19">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" s="18" t="s">
+        <v>2664</v>
+      </c>
+      <c r="B291" s="19">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" s="18" t="s">
+        <v>2714</v>
+      </c>
+      <c r="B292" s="19">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" s="18" t="s">
+        <v>2665</v>
+      </c>
+      <c r="B293" s="19">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" s="18" t="s">
+        <v>2879</v>
+      </c>
+      <c r="B294" s="19">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" s="18" t="s">
+        <v>2707</v>
+      </c>
+      <c r="B295" s="19">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" s="18" t="s">
+        <v>2852</v>
+      </c>
+      <c r="B296" s="19">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" s="18" t="s">
+        <v>2851</v>
+      </c>
+      <c r="B297" s="19">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" s="18" t="s">
+        <v>2965</v>
+      </c>
+      <c r="B298" s="19">
+        <v>7932</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" s="18" t="s">
+        <v>2709</v>
+      </c>
+      <c r="B299" s="19">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" s="18" t="s">
+        <v>2666</v>
+      </c>
+      <c r="B300" s="19">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" s="18" t="s">
+        <v>2997</v>
+      </c>
+      <c r="B301" s="19">
+        <v>8567333</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" s="18" t="s">
+        <v>2668</v>
+      </c>
+      <c r="B302" s="19">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" s="18" t="s">
+        <v>2667</v>
+      </c>
+      <c r="B303" s="19">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" s="18" t="s">
+        <v>2853</v>
+      </c>
+      <c r="B304" s="19">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" s="18" t="s">
+        <v>2998</v>
+      </c>
+      <c r="B305" s="19">
+        <v>8714133</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" s="18" t="s">
+        <v>2854</v>
+      </c>
+      <c r="B306" s="19">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" s="18" t="s">
+        <v>2855</v>
+      </c>
+      <c r="B307" s="19">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" s="18" t="s">
+        <v>2669</v>
+      </c>
+      <c r="B308" s="19">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309" s="18" t="s">
+        <v>2710</v>
+      </c>
+      <c r="B309" s="19">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" s="18" t="s">
+        <v>2670</v>
+      </c>
+      <c r="B310" s="19">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311" s="18" t="s">
+        <v>2999</v>
+      </c>
+      <c r="B311" s="19">
+        <v>9643703</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" s="18" t="s">
+        <v>2671</v>
+      </c>
+      <c r="B312" s="19">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" s="18" t="s">
+        <v>2856</v>
+      </c>
+      <c r="B313" s="19">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" s="18" t="s">
+        <v>2732</v>
+      </c>
+      <c r="B314" s="19">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" s="18" t="s">
+        <v>2706</v>
+      </c>
+      <c r="B315" s="19">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" s="18" t="s">
+        <v>2672</v>
+      </c>
+      <c r="B316" s="19">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" s="18" t="s">
+        <v>2857</v>
+      </c>
+      <c r="B317" s="19">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" s="18" t="s">
+        <v>2673</v>
+      </c>
+      <c r="B318" s="19">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" s="18" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B319" s="19">
+        <v>84783</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" s="18" t="s">
+        <v>2858</v>
+      </c>
+      <c r="B320" s="19">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" s="18" t="s">
+        <v>2674</v>
+      </c>
+      <c r="B321" s="19">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" s="18" t="s">
+        <v>2675</v>
+      </c>
+      <c r="B322" s="19">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" s="18" t="s">
+        <v>2676</v>
+      </c>
+      <c r="B323" s="19">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" s="18" t="s">
+        <v>2677</v>
+      </c>
+      <c r="B324" s="19">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" s="18" t="s">
+        <v>2678</v>
+      </c>
+      <c r="B325" s="19">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" s="18" t="s">
+        <v>2679</v>
+      </c>
+      <c r="B326" s="19">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" s="18" t="s">
+        <v>2680</v>
+      </c>
+      <c r="B327" s="19">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" s="18" t="s">
+        <v>2681</v>
+      </c>
+      <c r="B328" s="19">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" s="18" t="s">
+        <v>2682</v>
+      </c>
+      <c r="B329" s="19">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" s="18" t="s">
+        <v>2683</v>
+      </c>
+      <c r="B330" s="19">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" s="18" t="s">
+        <v>2876</v>
+      </c>
+      <c r="B331" s="19">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" s="18" t="s">
+        <v>2684</v>
+      </c>
+      <c r="B332" s="19">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" s="18" t="s">
+        <v>2685</v>
+      </c>
+      <c r="B333" s="19">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" s="18" t="s">
+        <v>2969</v>
+      </c>
+      <c r="B334" s="19">
+        <v>9933</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" s="18" t="s">
+        <v>2859</v>
+      </c>
+      <c r="B335" s="19">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" s="18" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B336" s="19">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" s="18" t="s">
+        <v>2860</v>
+      </c>
+      <c r="B337" s="19">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" s="18" t="s">
+        <v>2687</v>
+      </c>
+      <c r="B338" s="19">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" s="18" t="s">
+        <v>2688</v>
+      </c>
+      <c r="B339" s="19">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" s="18" t="s">
+        <v>2689</v>
+      </c>
+      <c r="B340" s="19">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" s="18" t="s">
+        <v>2821</v>
+      </c>
+      <c r="B341" s="19">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" s="18" t="s">
+        <v>2690</v>
+      </c>
+      <c r="B342" s="19">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" s="18" t="s">
+        <v>2863</v>
+      </c>
+      <c r="B343" s="19">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" s="18" t="s">
+        <v>2691</v>
+      </c>
+      <c r="B344" s="19">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" s="18" t="s">
+        <v>2692</v>
+      </c>
+      <c r="B345" s="19">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" s="18" t="s">
+        <v>3003</v>
+      </c>
+      <c r="B346" s="19">
+        <v>75077404</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" s="18" t="s">
+        <v>3004</v>
+      </c>
+      <c r="B347" s="19">
+        <v>80863204</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" s="18" t="s">
+        <v>2880</v>
+      </c>
+      <c r="B348" s="19">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" s="18" t="s">
+        <v>2968</v>
+      </c>
+      <c r="B349" s="19">
+        <v>9144</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" s="18" t="s">
+        <v>2721</v>
+      </c>
+      <c r="B350" s="19">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" s="18" t="s">
+        <v>2881</v>
+      </c>
+      <c r="B351" s="19">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" s="18" t="s">
+        <v>2882</v>
+      </c>
+      <c r="B352" s="19">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" s="18" t="s">
+        <v>2883</v>
+      </c>
+      <c r="B353" s="19">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" s="18" t="s">
+        <v>2713</v>
+      </c>
+      <c r="B354" s="19">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" s="18" t="s">
+        <v>2725</v>
+      </c>
+      <c r="B355" s="19">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" s="18" t="s">
+        <v>2729</v>
+      </c>
+      <c r="B356" s="19">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" s="18" t="s">
+        <v>2760</v>
+      </c>
+      <c r="B357" s="19">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" s="18" t="s">
+        <v>2693</v>
+      </c>
+      <c r="B358" s="19">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" s="18" t="s">
+        <v>2963</v>
+      </c>
+      <c r="B359" s="19">
+        <v>7836</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" s="18" t="s">
+        <v>2705</v>
+      </c>
+      <c r="B360" s="19">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" s="18" t="s">
+        <v>2694</v>
+      </c>
+      <c r="B361" s="19">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" s="18" t="s">
+        <v>2695</v>
+      </c>
+      <c r="B362" s="19">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" s="18" t="s">
+        <v>2696</v>
+      </c>
+      <c r="B363" s="19">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" s="18" t="s">
+        <v>3008</v>
+      </c>
+      <c r="B364" s="19">
+        <v>1220916237</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" s="18" t="s">
+        <v>2697</v>
+      </c>
+      <c r="B365" s="19">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" s="18" t="s">
+        <v>2806</v>
+      </c>
+      <c r="B366" s="19">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" s="18" t="s">
+        <v>2874</v>
+      </c>
+      <c r="B367" s="19">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" s="18" t="s">
+        <v>2875</v>
+      </c>
+      <c r="B368" s="19">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" s="18" t="s">
+        <v>2967</v>
+      </c>
+      <c r="B369" s="19">
+        <v>9079</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" s="18" t="s">
+        <v>2773</v>
+      </c>
+      <c r="B370" s="19">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="18" t="s">
+        <v>2805</v>
+      </c>
+      <c r="B371" s="19">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" s="18" t="s">
+        <v>2724</v>
+      </c>
+      <c r="B372" s="19">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" s="18" t="s">
+        <v>2861</v>
+      </c>
+      <c r="B373" s="19">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" s="18" t="s">
+        <v>2862</v>
+      </c>
+      <c r="B374" s="19">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" s="18" t="s">
+        <v>2884</v>
+      </c>
+      <c r="B375" s="19">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" s="18" t="s">
+        <v>2885</v>
+      </c>
+      <c r="B376" s="19">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" s="18" t="s">
+        <v>2716</v>
+      </c>
+      <c r="B377" s="19">
+        <v>753</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B377">
+    <sortState ref="A2:B377">
+      <sortCondition ref="A1:A377"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feature(resources/tdupe) : [ENGTYPES] update working copy and database with new engine types
</commit_message>
<xml_diff>
--- a/resources/physics/tdupe/workingCopy.xlsx
+++ b/resources/physics/tdupe/workingCopy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="carlist" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,14 @@
     <sheet name="hud" sheetId="3" r:id="rId3"/>
     <sheet name="rims" sheetId="4" r:id="rId4"/>
     <sheet name="brandNames" sheetId="5" r:id="rId5"/>
+    <sheet name="enginetypes" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">brandNames!$A$1:$B$377</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">carlist!$A$1:$B$300</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">hud!$A$1:$B$267</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">rims!$A$1:$B$299</definedName>
+    <definedName name="enginetypes">enginetypes!$A$1:$B$14</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4356" uniqueCount="3029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4380" uniqueCount="3051">
   <si>
     <t>Reference</t>
   </si>
@@ -9121,19 +9123,92 @@
   </si>
   <si>
     <t>FERRARI F40 Prime</t>
+  </si>
+  <si>
+    <t>W12</t>
+  </si>
+  <si>
+    <t>Flathead 4 Cylinder</t>
+  </si>
+  <si>
+    <t>V12</t>
+  </si>
+  <si>
+    <t>V10</t>
+  </si>
+  <si>
+    <t>V6</t>
+  </si>
+  <si>
+    <t>V16</t>
+  </si>
+  <si>
+    <t>Flathead 6 Cylinder</t>
+  </si>
+  <si>
+    <t>3 Cylinder Inline</t>
+  </si>
+  <si>
+    <t>4 Cylinder Inline</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>V8</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>6 Cylinder Inline</t>
+  </si>
+  <si>
+    <t>5 Cylinder Inline</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>W16</t>
+  </si>
+  <si>
+    <t>Pure Electric</t>
+  </si>
+  <si>
+    <t>Hybrid 3 Cylinder Inline</t>
+  </si>
+  <si>
+    <t>Hybrid V6</t>
+  </si>
+  <si>
+    <t>Hybrid V8</t>
+  </si>
+  <si>
+    <t>Hybrid V10</t>
+  </si>
+  <si>
+    <t>Hybrid V12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -9228,14 +9303,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -9244,15 +9320,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -9262,23 +9338,25 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="3"/>
     <cellStyle name="Texte explicatif" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9655,11 +9733,11 @@
       <selection activeCell="B421" sqref="B421:B461"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.875"/>
-    <col min="2" max="2" width="46.75"/>
-    <col min="3" max="1025" width="10.625"/>
+    <col min="1" max="1" width="13.85546875"/>
+    <col min="2" max="2" width="46.7109375"/>
+    <col min="3" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -14637,12 +14715,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C619"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.125" style="4"/>
-    <col min="2" max="3" width="13.875" style="4"/>
+    <col min="1" max="1" width="42.140625" style="4"/>
+    <col min="2" max="3" width="13.85546875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -16097,7 +16175,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>3016</v>
       </c>
@@ -21467,10 +21545,10 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45"/>
-    <col min="2" max="2" width="12.375" style="7"/>
+    <col min="2" max="2" width="12.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -26188,11 +26266,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.125"/>
-    <col min="2" max="2" width="13.875" style="7"/>
-    <col min="3" max="1025" width="10.625"/>
+    <col min="1" max="1" width="56.140625"/>
+    <col min="2" max="2" width="13.85546875" style="7"/>
+    <col min="3" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -31162,15 +31240,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B377"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.75" style="15" customWidth="1"/>
-    <col min="2" max="2" width="13.875" style="15" customWidth="1"/>
-    <col min="3" max="16384" width="9.125" style="15"/>
+    <col min="1" max="1" width="35.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="15" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -34197,4 +34273,208 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3041</v>
+      </c>
+      <c r="B2" s="19">
+        <v>543709</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3040</v>
+      </c>
+      <c r="B3" s="19">
+        <v>544709</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>3039</v>
+      </c>
+      <c r="B4" s="19">
+        <v>553709</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>3038</v>
+      </c>
+      <c r="B5" s="19">
+        <v>554709</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>3037</v>
+      </c>
+      <c r="B6" s="19">
+        <v>563709</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>3036</v>
+      </c>
+      <c r="B7" s="19">
+        <v>564709</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>3035</v>
+      </c>
+      <c r="B8" s="19">
+        <v>573709</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>3034</v>
+      </c>
+      <c r="B9" s="19">
+        <v>574709</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>3033</v>
+      </c>
+      <c r="B10" s="19">
+        <v>583709</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>3032</v>
+      </c>
+      <c r="B11" s="19">
+        <v>593709</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>3031</v>
+      </c>
+      <c r="B12" s="19">
+        <v>603709</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>3030</v>
+      </c>
+      <c r="B13" s="19">
+        <v>613709</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>3029</v>
+      </c>
+      <c r="B14" s="19">
+        <v>623709</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>3042</v>
+      </c>
+      <c r="B15" s="19">
+        <v>633709</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>3043</v>
+      </c>
+      <c r="B16" s="19">
+        <v>643709</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>3044</v>
+      </c>
+      <c r="B17" s="19">
+        <v>653709</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>3045</v>
+      </c>
+      <c r="B18" s="19">
+        <v>663709</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>3046</v>
+      </c>
+      <c r="B19" s="19">
+        <v>673709</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>3047</v>
+      </c>
+      <c r="B20" s="19">
+        <v>683709</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>3048</v>
+      </c>
+      <c r="B21" s="19">
+        <v>693709</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>3049</v>
+      </c>
+      <c r="B22" s="19">
+        <v>703709</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>3050</v>
+      </c>
+      <c r="B23" s="19">
+        <v>713709</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>